<commit_message>
Brazillian ECommerce Dataset REmoved
</commit_message>
<xml_diff>
--- a/Testing Knowledge on Datasets.xlsx
+++ b/Testing Knowledge on Datasets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysite.wellpoint.com/personal/ag78400_ad_wellpoint_com/Documents/machine_learning_basics/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{983037BC-B137-4940-850A-A93F3805A364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{983037BC-B137-4940-850A-A93F3805A364}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1C47D17-2331-5447-B69F-D4A42554E3C6}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="14400" xr2:uid="{2C2556B2-59EB-1246-B9D0-E522B122FFA2}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="23040" windowHeight="13940" xr2:uid="{2C2556B2-59EB-1246-B9D0-E522B122FFA2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -363,13 +363,13 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,14 +689,14 @@
   <dimension ref="A1:O62"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" customWidth="1"/>
     <col min="2" max="2" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
@@ -721,11 +721,11 @@
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
       <c r="L1" s="30"/>
-      <c r="M1" s="33"/>
-      <c r="N1" s="31" t="s">
+      <c r="M1" s="31"/>
+      <c r="N1" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="32"/>
+      <c r="O1" s="33"/>
     </row>
     <row r="2" spans="1:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">

</xml_diff>